<commit_message>
Changes related to data
</commit_message>
<xml_diff>
--- a/Shareskill/ExcelData/TestData.xlsx
+++ b/Shareskill/ExcelData/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test_Automation\Shareskill\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arjun\Documents\GitHub\Competition\Shareskill\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Url</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Credit</t>
   </si>
   <si>
-    <t>WorkSample</t>
-  </si>
-  <si>
     <t>Software Tester</t>
   </si>
   <si>
@@ -156,13 +153,49 @@
     <t>0300PM</t>
   </si>
   <si>
-    <t>C:\\Users\\arjun\\Desktop\\projects.txt</t>
-  </si>
-  <si>
     <t>StartDate</t>
   </si>
   <si>
     <t>EndDate</t>
+  </si>
+  <si>
+    <t>Location Type</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>CategoryId</t>
+  </si>
+  <si>
+    <t>Programming &amp; Tech</t>
+  </si>
+  <si>
+    <t>SubcategoryId</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Service Type</t>
+  </si>
+  <si>
+    <t>Skill Trade</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>cooking</t>
+  </si>
+  <si>
+    <t>Hourlybasis</t>
   </si>
 </sst>
 </file>
@@ -631,23 +664,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="9" max="9" width="44.42578125" customWidth="1"/>
+    <col min="3" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="10" width="22.140625" customWidth="1"/>
+    <col min="11" max="13" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -655,54 +688,90 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H2">
+        <v>17082019</v>
+      </c>
+      <c r="I2">
+        <v>23082019</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2">
-        <v>17082019</v>
-      </c>
-      <c r="E2">
-        <v>23082019</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2">
+      <c r="M2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
-        <v>44</v>
+      <c r="O2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made after review
</commit_message>
<xml_diff>
--- a/Shareskill/ExcelData/TestData.xlsx
+++ b/Shareskill/ExcelData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arjun\Documents\GitHub\Competition\Shareskill\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test_Automation\Shareskill\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>Url</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Hourlybasis</t>
+  </si>
+  <si>
+    <t>Skill-exchange</t>
   </si>
 </sst>
 </file>
@@ -666,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +765,7 @@
         <v>42</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="M2" t="s">
         <v>56</v>

</xml_diff>